<commit_message>
update tusbung harian lagi
</commit_message>
<xml_diff>
--- a/tgl 21 Manokwari.xlsx
+++ b/tgl 21 Manokwari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT APPS\billman advance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE81EF4D-9C99-4312-9C34-B234AF5FEA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D9F3F0-6E51-4BB9-A5D1-D3347803B0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D02473EF-0945-4B60-9DE6-F85A8A0EE341}"/>
   </bookViews>
@@ -7088,10 +7088,14 @@
   <dimension ref="A1:P762"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P762"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="31.5">
       <c r="A1" s="1" t="s">
@@ -18997,7 +19001,7 @@
       </c>
       <c r="K257" s="8"/>
       <c r="L257" s="9">
-        <f t="shared" ref="L257:L511" si="1">COUNTA(M257)</f>
+        <f t="shared" ref="L257:L484" si="1">COUNTA(M257)</f>
         <v>0</v>
       </c>
       <c r="M257" s="10"/>
@@ -29515,7 +29519,7 @@
       </c>
       <c r="K485" s="8"/>
       <c r="L485" s="9">
-        <f>COUNTA(M485)</f>
+        <f t="shared" ref="L485:L516" si="2">COUNTA(M485)</f>
         <v>0</v>
       </c>
       <c r="M485" s="14"/>
@@ -29560,7 +29564,7 @@
       </c>
       <c r="K486" s="8"/>
       <c r="L486" s="9">
-        <f>COUNTA(M486)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M486" s="10" t="s">
@@ -29607,7 +29611,7 @@
       </c>
       <c r="K487" s="8"/>
       <c r="L487" s="9">
-        <f>COUNTA(M487)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M487" s="12" t="s">
@@ -29654,7 +29658,7 @@
       </c>
       <c r="K488" s="8"/>
       <c r="L488" s="9">
-        <f>COUNTA(M488)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M488" s="12" t="s">
@@ -29701,7 +29705,7 @@
       </c>
       <c r="K489" s="8"/>
       <c r="L489" s="9">
-        <f>COUNTA(M489)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M489" s="10" t="s">
@@ -29748,7 +29752,7 @@
       </c>
       <c r="K490" s="8"/>
       <c r="L490" s="9">
-        <f>COUNTA(M490)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M490" s="10" t="s">
@@ -29795,7 +29799,7 @@
       </c>
       <c r="K491" s="8"/>
       <c r="L491" s="9">
-        <f>COUNTA(M491)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M491" s="10" t="s">
@@ -29842,7 +29846,7 @@
       </c>
       <c r="K492" s="8"/>
       <c r="L492" s="9">
-        <f>COUNTA(M492)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M492" s="14"/>
@@ -29887,7 +29891,7 @@
       </c>
       <c r="K493" s="8"/>
       <c r="L493" s="9">
-        <f>COUNTA(M493)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M493" s="10" t="s">
@@ -29934,7 +29938,7 @@
       </c>
       <c r="K494" s="8"/>
       <c r="L494" s="9">
-        <f>COUNTA(M494)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M494" s="12" t="s">
@@ -29981,7 +29985,7 @@
       </c>
       <c r="K495" s="8"/>
       <c r="L495" s="9">
-        <f>COUNTA(M495)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M495" s="10"/>
@@ -30026,7 +30030,7 @@
       </c>
       <c r="K496" s="8"/>
       <c r="L496" s="9">
-        <f>COUNTA(M496)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M496" s="12" t="s">
@@ -30073,7 +30077,7 @@
       </c>
       <c r="K497" s="8"/>
       <c r="L497" s="9">
-        <f>COUNTA(M497)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M497" s="12"/>
@@ -30118,7 +30122,7 @@
       </c>
       <c r="K498" s="8"/>
       <c r="L498" s="9">
-        <f>COUNTA(M498)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M498" s="10" t="s">
@@ -30165,7 +30169,7 @@
       </c>
       <c r="K499" s="8"/>
       <c r="L499" s="9">
-        <f>COUNTA(M499)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M499" s="10" t="s">
@@ -30212,7 +30216,7 @@
       </c>
       <c r="K500" s="8"/>
       <c r="L500" s="9">
-        <f>COUNTA(M500)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M500" s="12" t="s">
@@ -30259,7 +30263,7 @@
       </c>
       <c r="K501" s="8"/>
       <c r="L501" s="9">
-        <f>COUNTA(M501)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M501" s="12" t="s">
@@ -30306,7 +30310,7 @@
       </c>
       <c r="K502" s="8"/>
       <c r="L502" s="9">
-        <f>COUNTA(M502)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M502" s="10" t="s">
@@ -30353,7 +30357,7 @@
       </c>
       <c r="K503" s="8"/>
       <c r="L503" s="9">
-        <f>COUNTA(M503)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M503" s="12"/>
@@ -30398,7 +30402,7 @@
       </c>
       <c r="K504" s="8"/>
       <c r="L504" s="9">
-        <f>COUNTA(M504)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M504" s="10" t="s">
@@ -30445,7 +30449,7 @@
       </c>
       <c r="K505" s="8"/>
       <c r="L505" s="9">
-        <f>COUNTA(M505)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M505" s="10" t="s">
@@ -30492,7 +30496,7 @@
       </c>
       <c r="K506" s="8"/>
       <c r="L506" s="9">
-        <f>COUNTA(M506)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M506" s="10" t="s">
@@ -30539,7 +30543,7 @@
       </c>
       <c r="K507" s="8"/>
       <c r="L507" s="9">
-        <f>COUNTA(M507)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M507" s="10" t="s">
@@ -30586,7 +30590,7 @@
       </c>
       <c r="K508" s="8"/>
       <c r="L508" s="9">
-        <f>COUNTA(M508)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M508" s="12" t="s">
@@ -30633,7 +30637,7 @@
       </c>
       <c r="K509" s="8"/>
       <c r="L509" s="9">
-        <f>COUNTA(M509)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M509" s="10" t="s">
@@ -30680,7 +30684,7 @@
       </c>
       <c r="K510" s="8"/>
       <c r="L510" s="9">
-        <f>COUNTA(M510)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M510" s="10" t="s">
@@ -30727,7 +30731,7 @@
       </c>
       <c r="K511" s="8"/>
       <c r="L511" s="9">
-        <f>COUNTA(M511)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M511" s="10" t="s">
@@ -30774,7 +30778,7 @@
       </c>
       <c r="K512" s="8"/>
       <c r="L512" s="9">
-        <f>COUNTA(M512)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M512" s="10" t="s">
@@ -30821,7 +30825,7 @@
       </c>
       <c r="K513" s="8"/>
       <c r="L513" s="9">
-        <f>COUNTA(M513)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M513" s="12" t="s">
@@ -30868,7 +30872,7 @@
       </c>
       <c r="K514" s="8"/>
       <c r="L514" s="9">
-        <f>COUNTA(M514)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M514" s="14" t="s">
@@ -30915,7 +30919,7 @@
       </c>
       <c r="K515" s="8"/>
       <c r="L515" s="9">
-        <f>COUNTA(M515)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M515" s="10" t="s">
@@ -30962,7 +30966,7 @@
       </c>
       <c r="K516" s="8"/>
       <c r="L516" s="9">
-        <f>COUNTA(M516)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M516" s="12" t="s">
@@ -31009,7 +31013,7 @@
       </c>
       <c r="K517" s="8"/>
       <c r="L517" s="9">
-        <f>COUNTA(M517)</f>
+        <f t="shared" ref="L517:L548" si="3">COUNTA(M517)</f>
         <v>1</v>
       </c>
       <c r="M517" s="12" t="s">
@@ -31056,7 +31060,7 @@
       </c>
       <c r="K518" s="8"/>
       <c r="L518" s="9">
-        <f>COUNTA(M518)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M518" s="14" t="s">
@@ -31103,7 +31107,7 @@
       </c>
       <c r="K519" s="8"/>
       <c r="L519" s="9">
-        <f>COUNTA(M519)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M519" s="12" t="s">
@@ -31150,7 +31154,7 @@
       </c>
       <c r="K520" s="8"/>
       <c r="L520" s="9">
-        <f>COUNTA(M520)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M520" s="10" t="s">
@@ -31197,7 +31201,7 @@
       </c>
       <c r="K521" s="8"/>
       <c r="L521" s="9">
-        <f>COUNTA(M521)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M521" s="12" t="s">
@@ -31244,7 +31248,7 @@
       </c>
       <c r="K522" s="8"/>
       <c r="L522" s="9">
-        <f>COUNTA(M522)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M522" s="10" t="s">
@@ -31291,7 +31295,7 @@
       </c>
       <c r="K523" s="8"/>
       <c r="L523" s="9">
-        <f>COUNTA(M523)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M523" s="10" t="s">
@@ -31338,7 +31342,7 @@
       </c>
       <c r="K524" s="8"/>
       <c r="L524" s="9">
-        <f>COUNTA(M524)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M524" s="12" t="s">
@@ -31385,7 +31389,7 @@
       </c>
       <c r="K525" s="8"/>
       <c r="L525" s="9">
-        <f>COUNTA(M525)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M525" s="10" t="s">
@@ -31432,7 +31436,7 @@
       </c>
       <c r="K526" s="8"/>
       <c r="L526" s="9">
-        <f>COUNTA(M526)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M526" s="10" t="s">
@@ -31479,7 +31483,7 @@
       </c>
       <c r="K527" s="8"/>
       <c r="L527" s="9">
-        <f>COUNTA(M527)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M527" s="10" t="s">
@@ -31526,7 +31530,7 @@
       </c>
       <c r="K528" s="8"/>
       <c r="L528" s="9">
-        <f>COUNTA(M528)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M528" s="10" t="s">
@@ -31573,7 +31577,7 @@
       </c>
       <c r="K529" s="8"/>
       <c r="L529" s="9">
-        <f>COUNTA(M529)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M529" s="10" t="s">
@@ -31620,7 +31624,7 @@
       </c>
       <c r="K530" s="8"/>
       <c r="L530" s="9">
-        <f>COUNTA(M530)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M530" s="12" t="s">
@@ -31667,7 +31671,7 @@
       </c>
       <c r="K531" s="8"/>
       <c r="L531" s="9">
-        <f>COUNTA(M531)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M531" s="12" t="s">
@@ -31714,7 +31718,7 @@
       </c>
       <c r="K532" s="8"/>
       <c r="L532" s="9">
-        <f>COUNTA(M532)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M532" s="14" t="s">
@@ -31761,7 +31765,7 @@
       </c>
       <c r="K533" s="8"/>
       <c r="L533" s="9">
-        <f>COUNTA(M533)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M533" s="12" t="s">
@@ -31808,7 +31812,7 @@
       </c>
       <c r="K534" s="8"/>
       <c r="L534" s="9">
-        <f>COUNTA(M534)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M534" s="14" t="s">
@@ -31855,7 +31859,7 @@
       </c>
       <c r="K535" s="8"/>
       <c r="L535" s="9">
-        <f>COUNTA(M535)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M535" s="10" t="s">
@@ -31902,7 +31906,7 @@
       </c>
       <c r="K536" s="8"/>
       <c r="L536" s="9">
-        <f>COUNTA(M536)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M536" s="12" t="s">
@@ -31949,7 +31953,7 @@
       </c>
       <c r="K537" s="8"/>
       <c r="L537" s="9">
-        <f>COUNTA(M537)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M537" s="10" t="s">
@@ -31996,7 +32000,7 @@
       </c>
       <c r="K538" s="8"/>
       <c r="L538" s="9">
-        <f>COUNTA(M538)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M538" s="10" t="s">
@@ -32043,7 +32047,7 @@
       </c>
       <c r="K539" s="8"/>
       <c r="L539" s="9">
-        <f>COUNTA(M539)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M539" s="10" t="s">
@@ -32090,7 +32094,7 @@
       </c>
       <c r="K540" s="8"/>
       <c r="L540" s="9">
-        <f>COUNTA(M540)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M540" s="14" t="s">
@@ -32137,7 +32141,7 @@
       </c>
       <c r="K541" s="8"/>
       <c r="L541" s="9">
-        <f>COUNTA(M541)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M541" s="10" t="s">
@@ -32184,7 +32188,7 @@
       </c>
       <c r="K542" s="8"/>
       <c r="L542" s="9">
-        <f>COUNTA(M542)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M542" s="12" t="s">
@@ -32231,7 +32235,7 @@
       </c>
       <c r="K543" s="8"/>
       <c r="L543" s="9">
-        <f>COUNTA(M543)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M543" s="12" t="s">
@@ -32278,7 +32282,7 @@
       </c>
       <c r="K544" s="8"/>
       <c r="L544" s="9">
-        <f>COUNTA(M544)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M544" s="12" t="s">
@@ -32325,7 +32329,7 @@
       </c>
       <c r="K545" s="8"/>
       <c r="L545" s="9">
-        <f>COUNTA(M545)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M545" s="10" t="s">
@@ -32372,7 +32376,7 @@
       </c>
       <c r="K546" s="8"/>
       <c r="L546" s="9">
-        <f>COUNTA(M546)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M546" s="12" t="s">
@@ -32419,7 +32423,7 @@
       </c>
       <c r="K547" s="8"/>
       <c r="L547" s="9">
-        <f>COUNTA(M547)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M547" s="12" t="s">
@@ -32466,7 +32470,7 @@
       </c>
       <c r="K548" s="8"/>
       <c r="L548" s="9">
-        <f>COUNTA(M548)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M548" s="12" t="s">
@@ -32513,7 +32517,7 @@
       </c>
       <c r="K549" s="8"/>
       <c r="L549" s="9">
-        <f>COUNTA(M549)</f>
+        <f t="shared" ref="L549:L580" si="4">COUNTA(M549)</f>
         <v>1</v>
       </c>
       <c r="M549" s="14" t="s">
@@ -32560,7 +32564,7 @@
       </c>
       <c r="K550" s="8"/>
       <c r="L550" s="9">
-        <f>COUNTA(M550)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M550" s="12" t="s">
@@ -32607,7 +32611,7 @@
       </c>
       <c r="K551" s="8"/>
       <c r="L551" s="9">
-        <f>COUNTA(M551)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M551" s="10" t="s">
@@ -32654,7 +32658,7 @@
       </c>
       <c r="K552" s="8"/>
       <c r="L552" s="9">
-        <f>COUNTA(M552)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M552" s="12" t="s">
@@ -32701,7 +32705,7 @@
       </c>
       <c r="K553" s="8"/>
       <c r="L553" s="9">
-        <f>COUNTA(M553)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M553" s="14" t="s">
@@ -32748,7 +32752,7 @@
       </c>
       <c r="K554" s="8"/>
       <c r="L554" s="9">
-        <f>COUNTA(M554)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M554" s="10" t="s">
@@ -32795,7 +32799,7 @@
       </c>
       <c r="K555" s="8"/>
       <c r="L555" s="9">
-        <f>COUNTA(M555)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M555" s="10" t="s">
@@ -32842,7 +32846,7 @@
       </c>
       <c r="K556" s="8"/>
       <c r="L556" s="9">
-        <f>COUNTA(M556)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M556" s="10" t="s">
@@ -32889,7 +32893,7 @@
       </c>
       <c r="K557" s="8"/>
       <c r="L557" s="9">
-        <f>COUNTA(M557)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M557" s="10" t="s">
@@ -32936,7 +32940,7 @@
       </c>
       <c r="K558" s="8"/>
       <c r="L558" s="9">
-        <f t="shared" ref="L558:L762" si="2">COUNTA(M558)</f>
+        <f t="shared" ref="L558:L762" si="5">COUNTA(M558)</f>
         <v>0</v>
       </c>
       <c r="M558" s="10"/>
@@ -32981,7 +32985,7 @@
       </c>
       <c r="K559" s="8"/>
       <c r="L559" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M559" s="10" t="s">
@@ -33028,7 +33032,7 @@
       </c>
       <c r="K560" s="8"/>
       <c r="L560" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M560" s="10" t="s">
@@ -33075,7 +33079,7 @@
       </c>
       <c r="K561" s="25"/>
       <c r="L561" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M561" s="10"/>
@@ -33120,7 +33124,7 @@
       </c>
       <c r="K562" s="8"/>
       <c r="L562" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M562" s="10" t="s">
@@ -33167,7 +33171,7 @@
       </c>
       <c r="K563" s="25"/>
       <c r="L563" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M563" s="10" t="s">
@@ -33214,7 +33218,7 @@
       </c>
       <c r="K564" s="25"/>
       <c r="L564" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M564" s="10"/>
@@ -33259,7 +33263,7 @@
       </c>
       <c r="K565" s="8"/>
       <c r="L565" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M565" s="10" t="s">
@@ -33306,7 +33310,7 @@
       </c>
       <c r="K566" s="8"/>
       <c r="L566" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M566" s="10" t="s">
@@ -33353,7 +33357,7 @@
       </c>
       <c r="K567" s="25"/>
       <c r="L567" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M567" s="10"/>
@@ -33398,7 +33402,7 @@
       </c>
       <c r="K568" s="25"/>
       <c r="L568" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M568" s="10"/>
@@ -33443,7 +33447,7 @@
       </c>
       <c r="K569" s="25"/>
       <c r="L569" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M569" s="10"/>
@@ -33488,7 +33492,7 @@
       </c>
       <c r="K570" s="8"/>
       <c r="L570" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M570" s="10"/>
@@ -33533,7 +33537,7 @@
       </c>
       <c r="K571" s="8"/>
       <c r="L571" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M571" s="10" t="s">
@@ -33580,7 +33584,7 @@
       </c>
       <c r="K572" s="25"/>
       <c r="L572" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M572" s="10"/>
@@ -33625,7 +33629,7 @@
       </c>
       <c r="K573" s="8"/>
       <c r="L573" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M573" s="12"/>
@@ -33670,7 +33674,7 @@
       </c>
       <c r="K574" s="8"/>
       <c r="L574" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M574" s="10" t="s">
@@ -33717,7 +33721,7 @@
       </c>
       <c r="K575" s="25"/>
       <c r="L575" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M575" s="10" t="s">
@@ -33764,7 +33768,7 @@
       </c>
       <c r="K576" s="25"/>
       <c r="L576" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M576" s="10"/>
@@ -33809,7 +33813,7 @@
       </c>
       <c r="K577" s="8"/>
       <c r="L577" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M577" s="10"/>
@@ -33854,7 +33858,7 @@
       </c>
       <c r="K578" s="8"/>
       <c r="L578" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M578" s="10" t="s">
@@ -33901,7 +33905,7 @@
       </c>
       <c r="K579" s="8"/>
       <c r="L579" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M579" s="10" t="s">
@@ -33948,7 +33952,7 @@
       </c>
       <c r="K580" s="8"/>
       <c r="L580" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M580" s="10"/>
@@ -33993,7 +33997,7 @@
       </c>
       <c r="K581" s="8"/>
       <c r="L581" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M581" s="10" t="s">
@@ -34040,7 +34044,7 @@
       </c>
       <c r="K582" s="25"/>
       <c r="L582" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M582" s="10"/>
@@ -34085,7 +34089,7 @@
       </c>
       <c r="K583" s="25"/>
       <c r="L583" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M583" s="10"/>
@@ -34130,7 +34134,7 @@
       </c>
       <c r="K584" s="8"/>
       <c r="L584" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M584" s="10" t="s">
@@ -34177,7 +34181,7 @@
       </c>
       <c r="K585" s="25"/>
       <c r="L585" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M585" s="10"/>
@@ -34222,7 +34226,7 @@
       </c>
       <c r="K586" s="8"/>
       <c r="L586" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M586" s="10" t="s">
@@ -34269,7 +34273,7 @@
       </c>
       <c r="K587" s="8"/>
       <c r="L587" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M587" s="10"/>
@@ -34314,7 +34318,7 @@
       </c>
       <c r="K588" s="25"/>
       <c r="L588" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M588" s="10"/>
@@ -34359,7 +34363,7 @@
       </c>
       <c r="K589" s="25"/>
       <c r="L589" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M589" s="10"/>
@@ -34404,7 +34408,7 @@
       </c>
       <c r="K590" s="8"/>
       <c r="L590" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M590" s="10"/>
@@ -34449,7 +34453,7 @@
       </c>
       <c r="K591" s="8"/>
       <c r="L591" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M591" s="10"/>
@@ -34494,7 +34498,7 @@
       </c>
       <c r="K592" s="8"/>
       <c r="L592" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M592" s="10"/>
@@ -34539,7 +34543,7 @@
       </c>
       <c r="K593" s="8"/>
       <c r="L593" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M593" s="10"/>
@@ -34584,7 +34588,7 @@
       </c>
       <c r="K594" s="8"/>
       <c r="L594" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M594" s="12"/>
@@ -34629,7 +34633,7 @@
       </c>
       <c r="K595" s="8"/>
       <c r="L595" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M595" s="10"/>
@@ -34674,7 +34678,7 @@
       </c>
       <c r="K596" s="25"/>
       <c r="L596" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M596" s="10" t="s">
@@ -34721,7 +34725,7 @@
       </c>
       <c r="K597" s="25"/>
       <c r="L597" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M597" s="10" t="s">
@@ -34768,7 +34772,7 @@
       </c>
       <c r="K598" s="8"/>
       <c r="L598" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M598" s="10"/>
@@ -34813,7 +34817,7 @@
       </c>
       <c r="K599" s="25"/>
       <c r="L599" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M599" s="10"/>
@@ -34858,7 +34862,7 @@
       </c>
       <c r="K600" s="8"/>
       <c r="L600" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M600" s="10"/>
@@ -34903,7 +34907,7 @@
       </c>
       <c r="K601" s="8"/>
       <c r="L601" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M601" s="14"/>
@@ -34948,7 +34952,7 @@
       </c>
       <c r="K602" s="8"/>
       <c r="L602" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M602" s="10"/>
@@ -34993,7 +34997,7 @@
       </c>
       <c r="K603" s="8"/>
       <c r="L603" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M603" s="10"/>
@@ -35038,7 +35042,7 @@
       </c>
       <c r="K604" s="8"/>
       <c r="L604" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M604" s="10"/>
@@ -35083,7 +35087,7 @@
       </c>
       <c r="K605" s="8"/>
       <c r="L605" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M605" s="10"/>
@@ -35128,7 +35132,7 @@
       </c>
       <c r="K606" s="8"/>
       <c r="L606" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M606" s="10"/>
@@ -35173,7 +35177,7 @@
       </c>
       <c r="K607" s="8"/>
       <c r="L607" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M607" s="10"/>
@@ -35218,7 +35222,7 @@
       </c>
       <c r="K608" s="8"/>
       <c r="L608" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M608" s="10"/>
@@ -35263,7 +35267,7 @@
       </c>
       <c r="K609" s="25"/>
       <c r="L609" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M609" s="10"/>
@@ -35308,7 +35312,7 @@
       </c>
       <c r="K610" s="8"/>
       <c r="L610" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M610" s="10"/>
@@ -35353,7 +35357,7 @@
       </c>
       <c r="K611" s="8"/>
       <c r="L611" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M611" s="10"/>
@@ -35398,7 +35402,7 @@
       </c>
       <c r="K612" s="25"/>
       <c r="L612" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M612" s="10"/>
@@ -35443,7 +35447,7 @@
       </c>
       <c r="K613" s="25"/>
       <c r="L613" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M613" s="10"/>
@@ -35488,7 +35492,7 @@
       </c>
       <c r="K614" s="25"/>
       <c r="L614" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M614" s="10"/>
@@ -35533,7 +35537,7 @@
       </c>
       <c r="K615" s="25"/>
       <c r="L615" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M615" s="10"/>
@@ -35578,7 +35582,7 @@
       </c>
       <c r="K616" s="25"/>
       <c r="L616" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M616" s="10"/>
@@ -35623,7 +35627,7 @@
       </c>
       <c r="K617" s="8"/>
       <c r="L617" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M617" s="10" t="s">
@@ -35670,7 +35674,7 @@
       </c>
       <c r="K618" s="8"/>
       <c r="L618" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M618" s="10" t="s">
@@ -35717,7 +35721,7 @@
       </c>
       <c r="K619" s="8"/>
       <c r="L619" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M619" s="10"/>
@@ -35762,7 +35766,7 @@
       </c>
       <c r="K620" s="8"/>
       <c r="L620" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M620" s="14"/>
@@ -35807,7 +35811,7 @@
       </c>
       <c r="K621" s="8"/>
       <c r="L621" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M621" s="10" t="s">
@@ -35854,7 +35858,7 @@
       </c>
       <c r="K622" s="8"/>
       <c r="L622" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M622" s="10" t="s">
@@ -35901,7 +35905,7 @@
       </c>
       <c r="K623" s="8"/>
       <c r="L623" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M623" s="10"/>
@@ -35946,7 +35950,7 @@
       </c>
       <c r="K624" s="8"/>
       <c r="L624" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M624" s="10"/>
@@ -35991,7 +35995,7 @@
       </c>
       <c r="K625" s="8"/>
       <c r="L625" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M625" s="10" t="s">
@@ -36038,7 +36042,7 @@
       </c>
       <c r="K626" s="8"/>
       <c r="L626" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M626" s="10" t="s">
@@ -36085,7 +36089,7 @@
       </c>
       <c r="K627" s="8"/>
       <c r="L627" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M627" s="10"/>
@@ -36130,7 +36134,7 @@
       </c>
       <c r="K628" s="25"/>
       <c r="L628" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M628" s="10"/>
@@ -36175,7 +36179,7 @@
       </c>
       <c r="K629" s="8"/>
       <c r="L629" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M629" s="10" t="s">
@@ -36222,7 +36226,7 @@
       </c>
       <c r="K630" s="8"/>
       <c r="L630" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M630" s="10" t="s">
@@ -36269,7 +36273,7 @@
       </c>
       <c r="K631" s="25"/>
       <c r="L631" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M631" s="10"/>
@@ -36314,7 +36318,7 @@
       </c>
       <c r="K632" s="8"/>
       <c r="L632" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M632" s="10" t="s">
@@ -36361,7 +36365,7 @@
       </c>
       <c r="K633" s="8"/>
       <c r="L633" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M633" s="10" t="s">
@@ -36408,7 +36412,7 @@
       </c>
       <c r="K634" s="8"/>
       <c r="L634" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M634" s="10" t="s">
@@ -36455,7 +36459,7 @@
       </c>
       <c r="K635" s="8"/>
       <c r="L635" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M635" s="12"/>
@@ -36500,7 +36504,7 @@
       </c>
       <c r="K636" s="8"/>
       <c r="L636" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M636" s="12"/>
@@ -36545,7 +36549,7 @@
       </c>
       <c r="K637" s="8"/>
       <c r="L637" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M637" s="12"/>
@@ -36590,7 +36594,7 @@
       </c>
       <c r="K638" s="8"/>
       <c r="L638" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M638" s="10" t="s">
@@ -36637,7 +36641,7 @@
       </c>
       <c r="K639" s="8"/>
       <c r="L639" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M639" s="12" t="s">
@@ -36684,7 +36688,7 @@
       </c>
       <c r="K640" s="8"/>
       <c r="L640" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M640" s="10" t="s">
@@ -36731,7 +36735,7 @@
       </c>
       <c r="K641" s="8"/>
       <c r="L641" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M641" s="10" t="s">
@@ -36778,7 +36782,7 @@
       </c>
       <c r="K642" s="8"/>
       <c r="L642" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M642" s="10"/>
@@ -36823,7 +36827,7 @@
       </c>
       <c r="K643" s="8"/>
       <c r="L643" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M643" s="10"/>
@@ -36868,7 +36872,7 @@
       </c>
       <c r="K644" s="8"/>
       <c r="L644" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M644" s="10" t="s">
@@ -36915,7 +36919,7 @@
       </c>
       <c r="K645" s="8"/>
       <c r="L645" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M645" s="10"/>
@@ -36960,7 +36964,7 @@
       </c>
       <c r="K646" s="8"/>
       <c r="L646" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M646" s="14"/>
@@ -37005,7 +37009,7 @@
       </c>
       <c r="K647" s="8"/>
       <c r="L647" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M647" s="10"/>
@@ -37050,7 +37054,7 @@
       </c>
       <c r="K648" s="8"/>
       <c r="L648" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M648" s="10" t="s">
@@ -37097,7 +37101,7 @@
       </c>
       <c r="K649" s="8"/>
       <c r="L649" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M649" s="10"/>
@@ -37142,7 +37146,7 @@
       </c>
       <c r="K650" s="8"/>
       <c r="L650" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M650" s="14"/>
@@ -37187,7 +37191,7 @@
       </c>
       <c r="K651" s="8"/>
       <c r="L651" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M651" s="12"/>
@@ -37232,7 +37236,7 @@
       </c>
       <c r="K652" s="8"/>
       <c r="L652" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M652" s="10"/>
@@ -37277,7 +37281,7 @@
       </c>
       <c r="K653" s="8"/>
       <c r="L653" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M653" s="12"/>
@@ -37322,7 +37326,7 @@
       </c>
       <c r="K654" s="8"/>
       <c r="L654" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M654" s="12"/>
@@ -37367,7 +37371,7 @@
       </c>
       <c r="K655" s="8"/>
       <c r="L655" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M655" s="14"/>
@@ -37412,7 +37416,7 @@
       </c>
       <c r="K656" s="8"/>
       <c r="L656" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M656" s="14"/>
@@ -37457,7 +37461,7 @@
       </c>
       <c r="K657" s="8"/>
       <c r="L657" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M657" s="12"/>
@@ -37502,7 +37506,7 @@
       </c>
       <c r="K658" s="8"/>
       <c r="L658" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M658" s="12" t="s">
@@ -37549,7 +37553,7 @@
       </c>
       <c r="K659" s="8"/>
       <c r="L659" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M659" s="10"/>
@@ -37594,7 +37598,7 @@
       </c>
       <c r="K660" s="8"/>
       <c r="L660" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M660" s="10" t="s">
@@ -37641,7 +37645,7 @@
       </c>
       <c r="K661" s="8"/>
       <c r="L661" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M661" s="10"/>
@@ -37686,7 +37690,7 @@
       </c>
       <c r="K662" s="8"/>
       <c r="L662" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M662" s="12"/>
@@ -37731,7 +37735,7 @@
       </c>
       <c r="K663" s="8"/>
       <c r="L663" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M663" s="10"/>
@@ -37776,7 +37780,7 @@
       </c>
       <c r="K664" s="8"/>
       <c r="L664" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M664" s="10" t="s">
@@ -37823,7 +37827,7 @@
       </c>
       <c r="K665" s="8"/>
       <c r="L665" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M665" s="12" t="s">
@@ -37870,7 +37874,7 @@
       </c>
       <c r="K666" s="8"/>
       <c r="L666" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M666" s="10" t="s">
@@ -37917,7 +37921,7 @@
       </c>
       <c r="K667" s="8"/>
       <c r="L667" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M667" s="10"/>
@@ -37962,7 +37966,7 @@
       </c>
       <c r="K668" s="8"/>
       <c r="L668" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M668" s="10" t="s">
@@ -38009,7 +38013,7 @@
       </c>
       <c r="K669" s="8"/>
       <c r="L669" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M669" s="10"/>
@@ -38054,7 +38058,7 @@
       </c>
       <c r="K670" s="8"/>
       <c r="L670" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M670" s="14"/>
@@ -38099,7 +38103,7 @@
       </c>
       <c r="K671" s="8"/>
       <c r="L671" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M671" s="10" t="s">
@@ -38146,7 +38150,7 @@
       </c>
       <c r="K672" s="8"/>
       <c r="L672" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M672" s="10" t="s">
@@ -38193,7 +38197,7 @@
       </c>
       <c r="K673" s="8"/>
       <c r="L673" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M673" s="10" t="s">
@@ -38240,7 +38244,7 @@
       </c>
       <c r="K674" s="8"/>
       <c r="L674" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M674" s="10" t="s">
@@ -38287,7 +38291,7 @@
       </c>
       <c r="K675" s="8"/>
       <c r="L675" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M675" s="10" t="s">
@@ -38334,7 +38338,7 @@
       </c>
       <c r="K676" s="8"/>
       <c r="L676" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M676" s="12" t="s">
@@ -38381,7 +38385,7 @@
       </c>
       <c r="K677" s="8"/>
       <c r="L677" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M677" s="10"/>
@@ -38426,7 +38430,7 @@
       </c>
       <c r="K678" s="8"/>
       <c r="L678" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M678" s="14"/>
@@ -38471,7 +38475,7 @@
       </c>
       <c r="K679" s="8"/>
       <c r="L679" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M679" s="10"/>
@@ -38516,7 +38520,7 @@
       </c>
       <c r="K680" s="8"/>
       <c r="L680" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M680" s="12" t="s">
@@ -38563,7 +38567,7 @@
       </c>
       <c r="K681" s="8"/>
       <c r="L681" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M681" s="10" t="s">
@@ -38610,7 +38614,7 @@
       </c>
       <c r="K682" s="8"/>
       <c r="L682" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M682" s="10" t="s">
@@ -38657,7 +38661,7 @@
       </c>
       <c r="K683" s="8"/>
       <c r="L683" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M683" s="14"/>
@@ -38702,7 +38706,7 @@
       </c>
       <c r="K684" s="8"/>
       <c r="L684" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M684" s="12"/>
@@ -38747,7 +38751,7 @@
       </c>
       <c r="K685" s="8"/>
       <c r="L685" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M685" s="10" t="s">
@@ -38794,7 +38798,7 @@
       </c>
       <c r="K686" s="8"/>
       <c r="L686" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M686" s="12"/>
@@ -38839,7 +38843,7 @@
       </c>
       <c r="K687" s="8"/>
       <c r="L687" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M687" s="12"/>
@@ -38884,7 +38888,7 @@
       </c>
       <c r="K688" s="8"/>
       <c r="L688" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M688" s="14"/>
@@ -38929,7 +38933,7 @@
       </c>
       <c r="K689" s="8"/>
       <c r="L689" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M689" s="12"/>
@@ -38974,7 +38978,7 @@
       </c>
       <c r="K690" s="8"/>
       <c r="L690" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M690" s="12"/>
@@ -39019,7 +39023,7 @@
       </c>
       <c r="K691" s="8"/>
       <c r="L691" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M691" s="10" t="s">
@@ -39066,7 +39070,7 @@
       </c>
       <c r="K692" s="8"/>
       <c r="L692" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M692" s="14"/>
@@ -39111,7 +39115,7 @@
       </c>
       <c r="K693" s="8"/>
       <c r="L693" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M693" s="10" t="s">
@@ -39158,7 +39162,7 @@
       </c>
       <c r="K694" s="8"/>
       <c r="L694" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M694" s="14"/>
@@ -39203,7 +39207,7 @@
       </c>
       <c r="K695" s="8"/>
       <c r="L695" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M695" s="12"/>
@@ -39248,7 +39252,7 @@
       </c>
       <c r="K696" s="8"/>
       <c r="L696" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M696" s="10" t="s">
@@ -39295,7 +39299,7 @@
       </c>
       <c r="K697" s="8"/>
       <c r="L697" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M697" s="10"/>
@@ -39340,7 +39344,7 @@
       </c>
       <c r="K698" s="8"/>
       <c r="L698" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M698" s="10"/>
@@ -39385,7 +39389,7 @@
       </c>
       <c r="K699" s="8"/>
       <c r="L699" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M699" s="10" t="s">
@@ -39432,7 +39436,7 @@
       </c>
       <c r="K700" s="8"/>
       <c r="L700" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M700" s="10" t="s">
@@ -39479,7 +39483,7 @@
       </c>
       <c r="K701" s="8"/>
       <c r="L701" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M701" s="10" t="s">
@@ -39526,7 +39530,7 @@
       </c>
       <c r="K702" s="8"/>
       <c r="L702" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M702" s="12" t="s">
@@ -39573,7 +39577,7 @@
       </c>
       <c r="K703" s="8"/>
       <c r="L703" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M703" s="10" t="s">
@@ -39620,7 +39624,7 @@
       </c>
       <c r="K704" s="8"/>
       <c r="L704" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M704" s="10" t="s">
@@ -39667,7 +39671,7 @@
       </c>
       <c r="K705" s="8"/>
       <c r="L705" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M705" s="12" t="s">
@@ -39714,7 +39718,7 @@
       </c>
       <c r="K706" s="8"/>
       <c r="L706" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M706" s="10" t="s">
@@ -39761,7 +39765,7 @@
       </c>
       <c r="K707" s="8"/>
       <c r="L707" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M707" s="10" t="s">
@@ -39808,7 +39812,7 @@
       </c>
       <c r="K708" s="8"/>
       <c r="L708" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M708" s="10" t="s">
@@ -39855,7 +39859,7 @@
       </c>
       <c r="K709" s="8"/>
       <c r="L709" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M709" s="10" t="s">
@@ -39902,7 +39906,7 @@
       </c>
       <c r="K710" s="8"/>
       <c r="L710" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M710" s="10"/>
@@ -39947,7 +39951,7 @@
       </c>
       <c r="K711" s="8"/>
       <c r="L711" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M711" s="10" t="s">
@@ -39994,7 +39998,7 @@
       </c>
       <c r="K712" s="8"/>
       <c r="L712" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M712" s="10" t="s">
@@ -40041,7 +40045,7 @@
       </c>
       <c r="K713" s="8"/>
       <c r="L713" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M713" s="10" t="s">
@@ -40088,7 +40092,7 @@
       </c>
       <c r="K714" s="8"/>
       <c r="L714" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M714" s="10" t="s">
@@ -40135,7 +40139,7 @@
       </c>
       <c r="K715" s="8"/>
       <c r="L715" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M715" s="10" t="s">
@@ -40182,7 +40186,7 @@
       </c>
       <c r="K716" s="8"/>
       <c r="L716" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M716" s="10" t="s">
@@ -40229,7 +40233,7 @@
       </c>
       <c r="K717" s="8"/>
       <c r="L717" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M717" s="10" t="s">
@@ -40276,7 +40280,7 @@
       </c>
       <c r="K718" s="8"/>
       <c r="L718" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M718" s="10" t="s">
@@ -40323,7 +40327,7 @@
       </c>
       <c r="K719" s="8"/>
       <c r="L719" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M719" s="10" t="s">
@@ -40370,7 +40374,7 @@
       </c>
       <c r="K720" s="8"/>
       <c r="L720" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M720" s="11"/>
@@ -40415,7 +40419,7 @@
       </c>
       <c r="K721" s="8"/>
       <c r="L721" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M721" s="10" t="s">
@@ -40462,7 +40466,7 @@
       </c>
       <c r="K722" s="8"/>
       <c r="L722" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M722" s="10" t="s">
@@ -40509,7 +40513,7 @@
       </c>
       <c r="K723" s="8"/>
       <c r="L723" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M723" s="10" t="s">
@@ -40556,7 +40560,7 @@
       </c>
       <c r="K724" s="8"/>
       <c r="L724" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M724" s="10" t="s">
@@ -40603,7 +40607,7 @@
       </c>
       <c r="K725" s="8"/>
       <c r="L725" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M725" s="12" t="s">
@@ -40650,7 +40654,7 @@
       </c>
       <c r="K726" s="8"/>
       <c r="L726" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M726" s="12"/>
@@ -40695,7 +40699,7 @@
       </c>
       <c r="K727" s="8"/>
       <c r="L727" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M727" s="12" t="s">
@@ -40742,7 +40746,7 @@
       </c>
       <c r="K728" s="8"/>
       <c r="L728" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M728" s="12" t="s">
@@ -40789,7 +40793,7 @@
       </c>
       <c r="K729" s="8"/>
       <c r="L729" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M729" s="10" t="s">
@@ -40836,7 +40840,7 @@
       </c>
       <c r="K730" s="8"/>
       <c r="L730" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M730" s="10"/>
@@ -40881,7 +40885,7 @@
       </c>
       <c r="K731" s="8"/>
       <c r="L731" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M731" s="10" t="s">
@@ -40928,7 +40932,7 @@
       </c>
       <c r="K732" s="8"/>
       <c r="L732" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M732" s="10" t="s">
@@ -40975,7 +40979,7 @@
       </c>
       <c r="K733" s="8"/>
       <c r="L733" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M733" s="12" t="s">
@@ -41022,7 +41026,7 @@
       </c>
       <c r="K734" s="8"/>
       <c r="L734" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M734" s="10" t="s">
@@ -41069,7 +41073,7 @@
       </c>
       <c r="K735" s="8"/>
       <c r="L735" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M735" s="12"/>
@@ -41114,7 +41118,7 @@
       </c>
       <c r="K736" s="8"/>
       <c r="L736" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M736" s="10" t="s">
@@ -41161,7 +41165,7 @@
       </c>
       <c r="K737" s="8"/>
       <c r="L737" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M737" s="10"/>
@@ -41206,7 +41210,7 @@
       </c>
       <c r="K738" s="8"/>
       <c r="L738" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M738" s="10" t="s">
@@ -41253,7 +41257,7 @@
       </c>
       <c r="K739" s="8"/>
       <c r="L739" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M739" s="10"/>
@@ -41298,7 +41302,7 @@
       </c>
       <c r="K740" s="8"/>
       <c r="L740" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M740" s="10" t="s">
@@ -41345,7 +41349,7 @@
       </c>
       <c r="K741" s="8"/>
       <c r="L741" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M741" s="10"/>
@@ -41390,7 +41394,7 @@
       </c>
       <c r="K742" s="8"/>
       <c r="L742" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M742" s="10" t="s">
@@ -41437,7 +41441,7 @@
       </c>
       <c r="K743" s="8"/>
       <c r="L743" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M743" s="10" t="s">
@@ -41484,7 +41488,7 @@
       </c>
       <c r="K744" s="8"/>
       <c r="L744" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M744" s="12"/>
@@ -41529,7 +41533,7 @@
       </c>
       <c r="K745" s="8"/>
       <c r="L745" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M745" s="10"/>
@@ -41574,7 +41578,7 @@
       </c>
       <c r="K746" s="8"/>
       <c r="L746" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M746" s="10"/>
@@ -41619,7 +41623,7 @@
       </c>
       <c r="K747" s="8"/>
       <c r="L747" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M747" s="10" t="s">
@@ -41666,7 +41670,7 @@
       </c>
       <c r="K748" s="8"/>
       <c r="L748" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M748" s="10" t="s">
@@ -41713,7 +41717,7 @@
       </c>
       <c r="K749" s="8"/>
       <c r="L749" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M749" s="12" t="s">
@@ -41760,7 +41764,7 @@
       </c>
       <c r="K750" s="8"/>
       <c r="L750" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M750" s="10" t="s">
@@ -41807,7 +41811,7 @@
       </c>
       <c r="K751" s="8"/>
       <c r="L751" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M751" s="10" t="s">
@@ -41854,7 +41858,7 @@
       </c>
       <c r="K752" s="8"/>
       <c r="L752" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M752" s="10" t="s">
@@ -41901,7 +41905,7 @@
       </c>
       <c r="K753" s="8"/>
       <c r="L753" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M753" s="10" t="s">
@@ -41948,7 +41952,7 @@
       </c>
       <c r="K754" s="8"/>
       <c r="L754" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M754" s="12" t="s">
@@ -41995,7 +41999,7 @@
       </c>
       <c r="K755" s="8"/>
       <c r="L755" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M755" s="10" t="s">
@@ -42042,7 +42046,7 @@
       </c>
       <c r="K756" s="8"/>
       <c r="L756" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M756" s="10"/>
@@ -42087,7 +42091,7 @@
       </c>
       <c r="K757" s="8"/>
       <c r="L757" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M757" s="10" t="s">
@@ -42134,7 +42138,7 @@
       </c>
       <c r="K758" s="8"/>
       <c r="L758" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M758" s="10" t="s">
@@ -42181,7 +42185,7 @@
       </c>
       <c r="K759" s="8"/>
       <c r="L759" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M759" s="12"/>
@@ -42226,7 +42230,7 @@
       </c>
       <c r="K760" s="8"/>
       <c r="L760" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M760" s="12" t="s">
@@ -42273,7 +42277,7 @@
       </c>
       <c r="K761" s="8"/>
       <c r="L761" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M761" s="10" t="s">
@@ -42320,7 +42324,7 @@
       </c>
       <c r="K762" s="8"/>
       <c r="L762" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M762" s="10"/>

</xml_diff>